<commit_message>
fig bug + update
update bussiness màn thêm nhiệm vụ nhân viên. bỏ cột ghi chú trong màn báo cáo tuyển dụng chấm dứt, thêm file xuất excel cho màn đăng kí nhiệm vụ nhân viên
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/CD_TD_Report.xlsx
+++ b/QUANGHANH2/excel/TCLD/CD_TD_Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -46,13 +46,16 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>TỔNG HỢP CÁC ĐƠN VỊ CHẤM DỨT, TUYỂN DỤNG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +65,14 @@
     </font>
     <font>
       <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -82,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -105,11 +116,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -118,6 +191,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -400,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,62 +512,89 @@
     <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="1" t="s">
+    <row r="4" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:I2"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>